<commit_message>
successful deployment of import_master_to_db with real data. extra code to handle data inconsistencies added. tests passing apart from test_get_project_milestones, which is still in development
</commit_message>
<xml_diff>
--- a/tests/resources/milestones_test_master_4_2018.xlsx
+++ b/tests/resources/milestones_test_master_4_2018.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="62">
   <si>
     <t xml:space="preserve">Project/Programme Name</t>
   </si>
@@ -146,6 +146,9 @@
   </si>
   <si>
     <t xml:space="preserve">The sea gets deeper the further you go into it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assurance MM1 DCA</t>
   </si>
   <si>
     <t xml:space="preserve">Project MM18</t>
@@ -413,7 +416,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H31" activeCellId="0" sqref="H31"/>
+      <selection pane="bottomRight" activeCell="K24" activeCellId="0" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -733,56 +736,46 @@
       <c r="A17" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>43</v>
-      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="4"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>46</v>
+      <c r="C18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="3" t="n">
-        <v>41153</v>
-      </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="3" t="n">
-        <v>38504</v>
-      </c>
-      <c r="E19" s="3" t="n">
-        <v>41789</v>
-      </c>
-      <c r="F19" s="3" t="n">
-        <v>41106</v>
+      <c r="E19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -792,9 +785,7 @@
       <c r="B20" s="3" t="n">
         <v>41153</v>
       </c>
-      <c r="C20" s="3" t="n">
-        <v>41548</v>
-      </c>
+      <c r="C20" s="2"/>
       <c r="D20" s="3" t="n">
         <v>38504</v>
       </c>
@@ -809,36 +800,38 @@
       <c r="A21" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B21" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E21" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F21" s="1" t="n">
-        <v>0</v>
+      <c r="B21" s="3" t="n">
+        <v>41153</v>
+      </c>
+      <c r="C21" s="3" t="n">
+        <v>41548</v>
+      </c>
+      <c r="D21" s="3" t="n">
+        <v>38504</v>
+      </c>
+      <c r="E21" s="3" t="n">
+        <v>41789</v>
+      </c>
+      <c r="F21" s="3" t="n">
+        <v>41106</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>21</v>
+      <c r="B22" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="C22" s="2"/>
-      <c r="D22" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>21</v>
+      <c r="D22" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -846,52 +839,69 @@
         <v>51</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>52</v>
+        <v>21</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="6" t="s">
-        <v>54</v>
-      </c>
       <c r="C24" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C25" s="1" t="s">
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D25" s="4"/>
-      <c r="E25" s="2"/>
+      <c r="C26" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26" s="4"/>
+      <c r="E26" s="2"/>
     </row>
-    <row r="1046591" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1046592" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1046593" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1046594" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
some refactoring of MilestoneData get_milestones() and intro of get_chart_info(). so testing of deployment. tests passing
</commit_message>
<xml_diff>
--- a/tests/resources/milestones_test_master_4_2018.xlsx
+++ b/tests/resources/milestones_test_master_4_2018.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="72">
   <si>
     <t xml:space="preserve">Project/Programme Name</t>
   </si>
@@ -206,6 +206,36 @@
   </si>
   <si>
     <t xml:space="preserve">HSMRPG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Re-baseline this quarter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Re-baseline ALB/Programme milestones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Re-baseline ALB/Programme cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Re-baseline ALB/Programme benefits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Re-baseline IPDC milestones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Re-baseline IPDC cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Re-baseline IPDC benefits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Re-baseline HMT milestones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Re-baseline HMT cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Re-baseline HMT benefits</t>
   </si>
 </sst>
 </file>
@@ -416,7 +446,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K24" activeCellId="0" sqref="K24"/>
+      <selection pane="bottomRight" activeCell="J27" activeCellId="0" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -901,6 +931,98 @@
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="2"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
     </row>
     <row r="1046592" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1046593" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
further work on schedule changes
</commit_message>
<xml_diff>
--- a/tests/resources/milestones_test_master_4_2018.xlsx
+++ b/tests/resources/milestones_test_master_4_2018.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="73">
   <si>
     <t xml:space="preserve">Project/Programme Name</t>
   </si>
@@ -236,6 +236,9 @@
   </si>
   <si>
     <t xml:space="preserve">Re-baseline HMT benefits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPDC approval point</t>
   </si>
 </sst>
 </file>
@@ -446,7 +449,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J27" activeCellId="0" sqref="J27"/>
+      <selection pane="bottomRight" activeCell="A37" activeCellId="0" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1023,6 +1026,11 @@
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="6" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="1046592" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1046593" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>